<commit_message>
reran tests in order to prove function
</commit_message>
<xml_diff>
--- a/Midterm-exam/evidence/spreadsheets/audit_results.xlsx
+++ b/Midterm-exam/evidence/spreadsheets/audit_results.xlsx
@@ -514,25 +514,25 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" t="n">
-        <v>12795.237</v>
+        <v>12856.3315</v>
       </c>
       <c r="E2" t="n">
-        <v>31465.02250000001</v>
+        <v>31319.10899999998</v>
       </c>
       <c r="F2" t="n">
-        <v>12795.237</v>
+        <v>12856.3315</v>
       </c>
       <c r="G2" t="n">
-        <v>5665601</v>
+        <v>5666949</v>
       </c>
       <c r="H2" t="n">
         <v>61</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1301930</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -566,22 +566,22 @@
         <v>59</v>
       </c>
       <c r="D3" t="n">
-        <v>5996.65155</v>
+        <v>5875.24775</v>
       </c>
       <c r="E3" t="n">
-        <v>11015.11532151794</v>
+        <v>10476.48368800354</v>
       </c>
       <c r="F3" t="n">
-        <v>6833.131294821926</v>
+        <v>6733.031759310616</v>
       </c>
       <c r="G3" t="n">
-        <v>1537116</v>
+        <v>1537104</v>
       </c>
       <c r="H3" t="n">
         <v>47</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>647102</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -612,25 +612,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D4" t="n">
-        <v>1621.90728</v>
+        <v>2406.10756</v>
       </c>
       <c r="E4" t="n">
-        <v>3931.573650000001</v>
+        <v>9846.369949999997</v>
       </c>
       <c r="F4" t="n">
-        <v>2970.047791766616</v>
+        <v>4477.799266667214</v>
       </c>
       <c r="G4" t="n">
-        <v>1183952</v>
+        <v>1183927</v>
       </c>
       <c r="H4" t="n">
         <v>63</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>758093</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -661,25 +661,25 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" t="n">
-        <v>2564.869</v>
+        <v>2536.668</v>
       </c>
       <c r="E5" t="n">
-        <v>10492.95598</v>
+        <v>10578.80974</v>
       </c>
       <c r="F5" t="n">
-        <v>5015.206219323737</v>
+        <v>4992.058988892054</v>
       </c>
       <c r="G5" t="n">
-        <v>1177532</v>
+        <v>1185604</v>
       </c>
       <c r="H5" t="n">
         <v>44</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>650597</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -710,25 +710,25 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6" t="n">
-        <v>4530.911</v>
+        <v>4745.114</v>
       </c>
       <c r="E6" t="n">
-        <v>5990.2405</v>
+        <v>6105.682</v>
       </c>
       <c r="F6" t="n">
-        <v>5543.975383193276</v>
+        <v>5671.082166716559</v>
       </c>
       <c r="G6" t="n">
-        <v>1395554</v>
+        <v>1432910</v>
       </c>
       <c r="H6" t="n">
         <v>39</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>770319</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -762,22 +762,22 @@
         <v>58</v>
       </c>
       <c r="D7" t="n">
-        <v>6298.486000000001</v>
+        <v>6319.682999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>13934.94</v>
+        <v>13982.259</v>
       </c>
       <c r="F7" t="n">
-        <v>7331.358312684789</v>
+        <v>7257.048709542826</v>
       </c>
       <c r="G7" t="n">
-        <v>3220407</v>
+        <v>3220404</v>
       </c>
       <c r="H7" t="n">
         <v>48</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>676829</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -808,25 +808,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" t="n">
-        <v>5972.036</v>
+        <v>5837.446</v>
       </c>
       <c r="E8" t="n">
-        <v>8448.07</v>
+        <v>8438.512999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>5972.036</v>
+        <v>5903.616913760536</v>
       </c>
       <c r="G8" t="n">
-        <v>1111231</v>
+        <v>1111324</v>
       </c>
       <c r="H8" t="n">
         <v>36</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>432208</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -857,25 +857,25 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="n">
-        <v>4571.074000000001</v>
+        <v>4632.223999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>5855.299</v>
+        <v>5789.358999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>5221.814010581244</v>
+        <v>4877.75103212671</v>
       </c>
       <c r="G9" t="n">
-        <v>1386085</v>
+        <v>1364378</v>
       </c>
       <c r="H9" t="n">
         <v>34</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>770338</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -906,25 +906,25 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" t="n">
-        <v>4499.7035</v>
+        <v>4759.752</v>
       </c>
       <c r="E10" t="n">
-        <v>6001.287000000001</v>
+        <v>6078.044</v>
       </c>
       <c r="F10" t="n">
-        <v>5290.181578410829</v>
+        <v>5501.910514819657</v>
       </c>
       <c r="G10" t="n">
-        <v>1494934</v>
+        <v>1516659</v>
       </c>
       <c r="H10" t="n">
         <v>39</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>770306</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -958,22 +958,22 @@
         <v>64</v>
       </c>
       <c r="D11" t="n">
-        <v>3347.801</v>
+        <v>3229.920000000001</v>
       </c>
       <c r="E11" t="n">
-        <v>10709.99</v>
+        <v>10672.751</v>
       </c>
       <c r="F11" t="n">
-        <v>5817.99042126072</v>
+        <v>5713.540492995829</v>
       </c>
       <c r="G11" t="n">
-        <v>3113165</v>
+        <v>3112740</v>
       </c>
       <c r="H11" t="n">
         <v>82</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>464810</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1004,25 +1004,25 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D12" t="n">
-        <v>2898.88148</v>
+        <v>2820.24266</v>
       </c>
       <c r="E12" t="n">
-        <v>6904.636912971801</v>
+        <v>6461.98022</v>
       </c>
       <c r="F12" t="n">
-        <v>5983.297218845533</v>
+        <v>4208.519949127516</v>
       </c>
       <c r="G12" t="n">
-        <v>966644</v>
+        <v>928329</v>
       </c>
       <c r="H12" t="n">
         <v>68</v>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>248099</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1053,25 +1053,25 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" t="n">
-        <v>8567.99194</v>
+        <v>9302.184999999999</v>
       </c>
       <c r="E13" t="n">
-        <v>15392.688</v>
+        <v>16804.97022</v>
       </c>
       <c r="F13" t="n">
-        <v>8567.99194</v>
+        <v>9302.184999999999</v>
       </c>
       <c r="G13" t="n">
-        <v>2305514</v>
+        <v>2556234</v>
       </c>
       <c r="H13" t="n">
         <v>59</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>830748</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1102,25 +1102,25 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D14" t="n">
-        <v>2434.154999999999</v>
+        <v>2475.844000000001</v>
       </c>
       <c r="E14" t="n">
-        <v>6983.5225</v>
+        <v>6634.818</v>
       </c>
       <c r="F14" t="n">
-        <v>2452.63587655792</v>
+        <v>2475.844000000001</v>
       </c>
       <c r="G14" t="n">
-        <v>1239150</v>
+        <v>1239153</v>
       </c>
       <c r="H14" t="n">
         <v>46</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>273758</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1151,25 +1151,25 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" t="n">
-        <v>4596.284</v>
+        <v>4557.028000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>5401.6</v>
+        <v>5759.991</v>
       </c>
       <c r="F15" t="n">
-        <v>5643.254968414647</v>
+        <v>5160.984846839408</v>
       </c>
       <c r="G15" t="n">
-        <v>1460002</v>
+        <v>1498904</v>
       </c>
       <c r="H15" t="n">
         <v>38</v>
       </c>
       <c r="I15" t="n">
-        <v>0</v>
+        <v>770322</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1200,25 +1200,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D16" t="n">
-        <v>4829.260499999999</v>
+        <v>4839.279</v>
       </c>
       <c r="E16" t="n">
-        <v>6573.932500000001</v>
+        <v>6519.782999999999</v>
       </c>
       <c r="F16" t="n">
-        <v>5579.952946391422</v>
+        <v>5347.843346807336</v>
       </c>
       <c r="G16" t="n">
-        <v>1724245</v>
+        <v>1708494</v>
       </c>
       <c r="H16" t="n">
         <v>51</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1109827</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1249,25 +1249,25 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" t="n">
-        <v>7900.891</v>
+        <v>6945.37916</v>
       </c>
       <c r="E17" t="n">
-        <v>17286.44724</v>
+        <v>16262.5585</v>
       </c>
       <c r="F17" t="n">
-        <v>7900.891</v>
+        <v>6945.37916</v>
       </c>
       <c r="G17" t="n">
-        <v>5742233</v>
+        <v>6238283</v>
       </c>
       <c r="H17" t="n">
         <v>96</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>757169</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1301,22 +1301,22 @@
         <v>59</v>
       </c>
       <c r="D18" t="n">
-        <v>5781.3825</v>
+        <v>6169.28</v>
       </c>
       <c r="E18" t="n">
-        <v>8068.339</v>
+        <v>8051.973999999999</v>
       </c>
       <c r="F18" t="n">
-        <v>5781.3825</v>
+        <v>6169.28</v>
       </c>
       <c r="G18" t="n">
-        <v>2485721</v>
+        <v>2485573</v>
       </c>
       <c r="H18" t="n">
         <v>47</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>1236728</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1347,25 +1347,25 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D19" t="n">
-        <v>14544.805</v>
+        <v>14623.8915</v>
       </c>
       <c r="E19" t="n">
-        <v>18775.42</v>
+        <v>19100.0175</v>
       </c>
       <c r="F19" t="n">
-        <v>14544.805</v>
+        <v>14623.8915</v>
       </c>
       <c r="G19" t="n">
-        <v>3158802</v>
+        <v>3158830</v>
       </c>
       <c r="H19" t="n">
         <v>68</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>1624491</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1396,25 +1396,25 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" t="n">
-        <v>8467.545999999998</v>
+        <v>8464.333999999999</v>
       </c>
       <c r="E20" t="n">
-        <v>23871.925</v>
+        <v>23901.5495</v>
       </c>
       <c r="F20" t="n">
-        <v>8843.175719509461</v>
+        <v>8464.333999999999</v>
       </c>
       <c r="G20" t="n">
-        <v>6750788</v>
+        <v>6750718</v>
       </c>
       <c r="H20" t="n">
         <v>50</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>602446</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1445,25 +1445,25 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" t="n">
-        <v>5815.897999999999</v>
+        <v>8840.423000000001</v>
       </c>
       <c r="E21" t="n">
-        <v>11223.6465</v>
+        <v>10867.421</v>
       </c>
       <c r="F21" t="n">
-        <v>6891.641652486893</v>
+        <v>8840.423000000001</v>
       </c>
       <c r="G21" t="n">
-        <v>1595060</v>
+        <v>1595016</v>
       </c>
       <c r="H21" t="n">
         <v>40</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>872009</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1494,25 +1494,25 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D22" t="n">
-        <v>2577.384</v>
+        <v>2771.625</v>
       </c>
       <c r="E22" t="n">
-        <v>5015.428</v>
+        <v>6564.225</v>
       </c>
       <c r="F22" t="n">
-        <v>3045.665209312721</v>
+        <v>3032.918283528135</v>
       </c>
       <c r="G22" t="n">
-        <v>868677</v>
+        <v>868685</v>
       </c>
       <c r="H22" t="n">
         <v>60</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>386492</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>62.95</v>
+        <v>61.62</v>
       </c>
     </row>
     <row r="3">
@@ -1579,7 +1579,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5743.48</v>
+        <v>5952.76</v>
       </c>
     </row>
     <row r="4">
@@ -1589,7 +1589,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>11111.53</v>
+        <v>11438.89</v>
       </c>
     </row>
     <row r="5">
@@ -1599,7 +1599,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6572.65</v>
+        <v>6597.89</v>
       </c>
     </row>
     <row r="6">
@@ -1619,7 +1619,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>759743.86</v>
       </c>
     </row>
     <row r="8">
@@ -1629,7 +1629,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.252</v>
+        <v>2.287</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Audit pipeline: median LH, green hosting, CO2 calc, CSV+charts+spreadsheets; add JSBytes; docs
</commit_message>
<xml_diff>
--- a/Midterm-exam/evidence/spreadsheets/audit_results.xlsx
+++ b/Midterm-exam/evidence/spreadsheets/audit_results.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,35 +468,50 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>TBT</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>CLS</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>PageWeightBytes</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Requests</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>JSBytes</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>GreenHosting</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>GreenHostName</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>CarbonTxt</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>CO2_SWD_g</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>CO2_OneByte_g</t>
         </is>
@@ -526,29 +541,36 @@
         <v>12856.3315</v>
       </c>
       <c r="G2" t="n">
+        <v>252</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>5666949</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>61</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>1301930</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>2.170386362921401</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1.647630423613</v>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>2.170902756648601</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.648022439537</v>
       </c>
     </row>
     <row r="3">
@@ -575,29 +597,36 @@
         <v>6733.031759310616</v>
       </c>
       <c r="G3" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
         <v>1537104</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>47</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>647102</v>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>0.5888405492424</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.4470133153079999</v>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O3" t="n">
+        <v>0.5888359522656</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.4470098255519999</v>
       </c>
     </row>
     <row r="4">
@@ -624,29 +653,40 @@
         <v>4477.799266667214</v>
       </c>
       <c r="G4" t="n">
+        <v>58</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.0068852206501101</v>
+      </c>
+      <c r="I4" t="n">
         <v>1183927</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>63</v>
       </c>
-      <c r="I4" t="n">
+      <c r="K4" t="n">
         <v>758093</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>0.4535499896928</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.344308632976</v>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Cloudflare</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O4" t="n">
+        <v>0.4535404126578</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.344301362651</v>
       </c>
     </row>
     <row r="5">
@@ -673,29 +713,40 @@
         <v>4992.058988892054</v>
       </c>
       <c r="G5" t="n">
+        <v>77</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>1185604</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>44</v>
       </c>
-      <c r="I5" t="n">
+      <c r="K5" t="n">
         <v>650597</v>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
-        <v>0.4510906071048</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.3424416135159999</v>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Cloudflare</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O5" t="n">
+        <v>0.4541828401656</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.344789056052</v>
       </c>
     </row>
     <row r="6">
@@ -722,29 +773,36 @@
         <v>5671.082166716559</v>
       </c>
       <c r="G6" t="n">
+        <v>177.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.0056225658040376</v>
+      </c>
+      <c r="I6" t="n">
         <v>1432910</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>39</v>
       </c>
-      <c r="I6" t="n">
+      <c r="K6" t="n">
         <v>770319</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L6" t="n">
-        <v>0.5346107800956</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.4058452454019999</v>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>0.548921168874</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.4167088558299999</v>
       </c>
     </row>
     <row r="7">
@@ -771,29 +829,36 @@
         <v>7257.048709542826</v>
       </c>
       <c r="G7" t="n">
+        <v>71.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
         <v>3220404</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>48</v>
       </c>
-      <c r="I7" t="n">
+      <c r="K7" t="n">
         <v>676829</v>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>1.2336780221298</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.936536220891</v>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O7" t="n">
+        <v>1.2336768728856</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.936535348452</v>
       </c>
     </row>
     <row r="8">
@@ -820,29 +885,36 @@
         <v>5903.616913760536</v>
       </c>
       <c r="G8" t="n">
+        <v>144</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
         <v>1111324</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>36</v>
       </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
         <v>432208</v>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>0.4256919272034</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.3231604208029999</v>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O8" t="n">
+        <v>0.4257275537736</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.3231874664119999</v>
       </c>
     </row>
     <row r="9">
@@ -869,29 +941,36 @@
         <v>4877.75103212671</v>
       </c>
       <c r="G9" t="n">
+        <v>194.5000000000009</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
         <v>1364378</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>34</v>
       </c>
-      <c r="I9" t="n">
+      <c r="K9" t="n">
         <v>770338</v>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L9" t="n">
-        <v>0.530983382319</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.4030915371049999</v>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O9" t="n">
+        <v>0.5226678343692001</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.3967788593139999</v>
       </c>
     </row>
     <row r="10">
@@ -918,29 +997,36 @@
         <v>5501.910514819657</v>
       </c>
       <c r="G10" t="n">
+        <v>175.5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>1516659</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>39</v>
       </c>
-      <c r="I10" t="n">
+      <c r="K10" t="n">
         <v>770306</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L10" t="n">
-        <v>0.5726814096276001</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.4347462413419999</v>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O10" t="n">
+        <v>0.5810038530426</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.4410641537669999</v>
       </c>
     </row>
     <row r="11">
@@ -967,29 +1053,40 @@
         <v>5713.540492995829</v>
       </c>
       <c r="G11" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0007589648594464</v>
+      </c>
+      <c r="I11" t="n">
         <v>3112740</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>82</v>
       </c>
-      <c r="I11" t="n">
+      <c r="K11" t="n">
         <v>464810</v>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L11" t="n">
-        <v>1.192595606631</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.9053488531449998</v>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>Sitevision AB</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O11" t="n">
+        <v>1.192432797036</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.9052252576199999</v>
       </c>
     </row>
     <row r="12">
@@ -1016,29 +1113,36 @@
         <v>4208.519949127516</v>
       </c>
       <c r="G12" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0592427032813799</v>
+      </c>
+      <c r="I12" t="n">
         <v>928329</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>68</v>
       </c>
-      <c r="I12" t="n">
+      <c r="K12" t="n">
         <v>248099</v>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>0.3703033368216</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.2811126415719999</v>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O12" t="n">
+        <v>0.3556255729806</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.269970141477</v>
       </c>
     </row>
     <row r="13">
@@ -1065,29 +1169,36 @@
         <v>9302.184999999999</v>
       </c>
       <c r="G13" t="n">
+        <v>131</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
         <v>2556234</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
         <v>59</v>
       </c>
-      <c r="I13" t="n">
+      <c r="K13" t="n">
         <v>830748</v>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>0.8831995308396001</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.6704734428819999</v>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O13" t="n">
+        <v>0.9792456994476</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.7433860782419999</v>
       </c>
     </row>
     <row r="14">
@@ -1114,29 +1225,40 @@
         <v>2475.844000000001</v>
       </c>
       <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.0038646982166687</v>
+      </c>
+      <c r="I14" t="n">
         <v>1239153</v>
       </c>
-      <c r="H14" t="n">
+      <c r="J14" t="n">
         <v>46</v>
       </c>
-      <c r="I14" t="n">
+      <c r="K14" t="n">
         <v>273758</v>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>0.4746953168100001</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.3603609289499999</v>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Sitevision AB</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O14" t="n">
+        <v>0.4746964660542</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.3603618013889999</v>
       </c>
     </row>
     <row r="15">
@@ -1163,29 +1285,36 @@
         <v>5160.984846839408</v>
       </c>
       <c r="G15" t="n">
+        <v>127.5000000000009</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
         <v>1498904</v>
       </c>
-      <c r="H15" t="n">
+      <c r="J15" t="n">
         <v>38</v>
       </c>
-      <c r="I15" t="n">
+      <c r="K15" t="n">
         <v>770322</v>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L15" t="n">
-        <v>0.5592996101628001</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.4245875616259999</v>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O15" t="n">
+        <v>0.5742022427855999</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.4359007689519999</v>
       </c>
     </row>
     <row r="16">
@@ -1212,29 +1341,36 @@
         <v>5347.843346807336</v>
       </c>
       <c r="G16" t="n">
+        <v>120.5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>1708494</v>
       </c>
-      <c r="H16" t="n">
+      <c r="J16" t="n">
         <v>51</v>
       </c>
-      <c r="I16" t="n">
+      <c r="K16" t="n">
         <v>1109827</v>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L16" t="n">
-        <v>0.660526188543</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.501432861185</v>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O16" t="n">
+        <v>0.6544922734116001</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.4968522656219999</v>
       </c>
     </row>
     <row r="17">
@@ -1261,29 +1397,36 @@
         <v>6945.37916</v>
       </c>
       <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
         <v>6238283</v>
       </c>
-      <c r="H17" t="n">
+      <c r="J17" t="n">
         <v>96</v>
       </c>
-      <c r="I17" t="n">
+      <c r="K17" t="n">
         <v>757169</v>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L17" t="n">
-        <v>2.1997426567662</v>
-      </c>
-      <c r="M17" t="n">
-        <v>1.669916005429</v>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O17" t="n">
+        <v>2.3897701852362</v>
+      </c>
+      <c r="P17" t="n">
+        <v>1.814173794079</v>
       </c>
     </row>
     <row r="18">
@@ -1310,29 +1453,36 @@
         <v>6169.28</v>
       </c>
       <c r="G18" t="n">
+        <v>133</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.0123655455877825</v>
+      </c>
+      <c r="I18" t="n">
         <v>2485573</v>
       </c>
-      <c r="H18" t="n">
+      <c r="J18" t="n">
         <v>47</v>
       </c>
-      <c r="I18" t="n">
+      <c r="K18" t="n">
         <v>1236728</v>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L18" t="n">
-        <v>0.9522334806893999</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.7228799811729999</v>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O18" t="n">
+        <v>0.9521767846422002</v>
+      </c>
+      <c r="P18" t="n">
+        <v>0.7228369408489999</v>
       </c>
     </row>
     <row r="19">
@@ -1359,29 +1509,36 @@
         <v>14623.8915</v>
       </c>
       <c r="G19" t="n">
+        <v>287.5</v>
+      </c>
+      <c r="H19" t="n">
+        <v>3.829323822311932e-05</v>
+      </c>
+      <c r="I19" t="n">
         <v>3158830</v>
       </c>
-      <c r="H19" t="n">
+      <c r="J19" t="n">
         <v>68</v>
       </c>
-      <c r="I19" t="n">
+      <c r="K19" t="n">
         <v>1624491</v>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L19" t="n">
-        <v>1.2100782924828</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0.918620686026</v>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O19" t="n">
+        <v>1.210089018762</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.91862882879</v>
       </c>
     </row>
     <row r="20">
@@ -1408,29 +1565,36 @@
         <v>8464.333999999999</v>
       </c>
       <c r="G20" t="n">
+        <v>90.49999999999818</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
         <v>6750718</v>
       </c>
-      <c r="H20" t="n">
+      <c r="J20" t="n">
         <v>50</v>
       </c>
-      <c r="I20" t="n">
+      <c r="K20" t="n">
         <v>602446</v>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L20" t="n">
-        <v>2.5861013181432</v>
-      </c>
-      <c r="M20" t="n">
-        <v>1.963216910644</v>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O20" t="n">
+        <v>2.586074502445201</v>
+      </c>
+      <c r="P20" t="n">
+        <v>1.963196553734</v>
       </c>
     </row>
     <row r="21">
@@ -1457,29 +1621,36 @@
         <v>8840.423000000001</v>
       </c>
       <c r="G21" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
         <v>1595016</v>
       </c>
-      <c r="H21" t="n">
+      <c r="J21" t="n">
         <v>40</v>
       </c>
-      <c r="I21" t="n">
+      <c r="K21" t="n">
         <v>872009</v>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L21" t="n">
-        <v>0.611037817884</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0.4638641837799999</v>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O21" t="n">
+        <v>0.6110209623024</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.4638513880079999</v>
       </c>
     </row>
     <row r="22">
@@ -1506,29 +1677,40 @@
         <v>3032.918283528135</v>
       </c>
       <c r="G22" t="n">
+        <v>49.99999999999909</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
         <v>868685</v>
       </c>
-      <c r="H22" t="n">
+      <c r="J22" t="n">
         <v>60</v>
       </c>
-      <c r="I22" t="n">
+      <c r="K22" t="n">
         <v>386492</v>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="L22" t="n">
-        <v>0.3327740013078</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0.2526225644009999</v>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>Sitevision AB</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="O22" t="n">
+        <v>0.332777065959</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.2526248909049999</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1605,51 +1787,71 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Avg_Requests</t>
+          <t>Avg_TBT_ms</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>53.14</v>
+        <v>104.43</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Avg_JSBytes</t>
+          <t>Avg_CLS</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>759743.86</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Avg_PageWeight_MB</t>
+          <t>Avg_Requests</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.287</v>
+        <v>53.14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Avg_CO2_SWD_g</t>
+          <t>Avg_JSBytes</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9045</v>
+        <v>759743.86</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Avg_PageWeight_MB</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2.287</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Avg_CO2_SWD_g</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9187</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>Avg_CO2_OneByte_g</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>0.6866</v>
+      <c r="B12" t="n">
+        <v>0.6974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>